<commit_message>
update cluster to 5
</commit_message>
<xml_diff>
--- a/dataset/processed/wordcount_by_cluster.xlsx
+++ b/dataset/processed/wordcount_by_cluster.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D161"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,15 +455,15 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>anggar</t>
+          <t>gizi</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
@@ -471,15 +471,15 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>rakyat</t>
+          <t>perintah</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
@@ -487,15 +487,15 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>bantu</t>
+          <t>anak</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -503,15 +503,15 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dana</t>
+          <t>indonesia</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -519,15 +519,15 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>hasil</t>
+          <t>menu</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -535,15 +535,15 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>daerah</t>
+          <t>rumah</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -551,15 +551,15 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>prabowo</t>
+          <t>anggar</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -567,15 +567,15 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>uang</t>
+          <t>sehat</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
@@ -583,15 +583,15 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>triliun</t>
+          <t>butuh</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -599,15 +599,15 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>presiden</t>
+          <t>bikin</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
@@ -615,15 +615,15 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>banget</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
@@ -631,15 +631,15 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>laksana</t>
+          <t>sekolah</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
@@ -647,15 +647,15 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>perintah</t>
+          <t>anakanak</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
@@ -663,15 +663,15 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>rp</t>
+          <t>tuju</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
@@ -679,15 +679,15 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>gas</t>
+          <t>daerah</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
@@ -695,15 +695,15 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>gizi</t>
+          <t>miskin</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18">
@@ -711,15 +711,15 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>pemda</t>
+          <t>dukung</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
@@ -727,15 +727,15 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>sekolah</t>
+          <t>kritik</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20">
@@ -743,15 +743,15 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>jalan</t>
+          <t>dana</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
@@ -759,15 +759,15 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>efisiensi</t>
+          <t>biar</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
@@ -779,11 +779,11 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>anak</t>
+          <t>udah</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
@@ -795,11 +795,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>menu</t>
+          <t>butuh</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
@@ -811,11 +811,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>perintah</t>
+          <t>gue</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
@@ -827,11 +827,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>si</t>
+          <t>anak</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
@@ -843,11 +843,11 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>video</t>
+          <t>sekolah</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
@@ -859,11 +859,11 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>sekolah</t>
+          <t>ribu</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
@@ -875,11 +875,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>azka</t>
+          <t>enak</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
@@ -891,11 +891,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>banget</t>
+          <t>lengkuas</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
@@ -907,11 +907,11 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>bikin</t>
+          <t>uang</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
@@ -923,11 +923,11 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>tu</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -939,11 +939,11 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>pake</t>
+          <t>bikin</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -955,11 +955,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>banding</t>
+          <t>anggar</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
@@ -971,11 +971,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>ni</t>
+          <t>gitu</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
@@ -987,11 +987,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>dapet</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -1003,11 +1003,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>vendor</t>
+          <t>nggak</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
@@ -1019,11 +1019,11 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>sih</t>
+          <t>orang</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
@@ -1035,11 +1035,11 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>nasi</t>
+          <t>hold</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1051,11 +1051,11 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>gua</t>
+          <t>wowo</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -1067,11 +1067,11 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>dipake</t>
+          <t>airdrop</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -1083,11 +1083,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>gue</t>
+          <t>hahahaduitny</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1095,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="B42" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1103,7 +1103,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43">
@@ -1111,15 +1111,15 @@
         <v>1</v>
       </c>
       <c r="B43" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>gue</t>
+          <t>bikin</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44">
@@ -1127,15 +1127,15 @@
         <v>2</v>
       </c>
       <c r="B44" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>bikin</t>
+          <t>si</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45">
@@ -1143,15 +1143,15 @@
         <v>3</v>
       </c>
       <c r="B45" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>utk</t>
+          <t>perintah</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46">
@@ -1159,15 +1159,15 @@
         <v>4</v>
       </c>
       <c r="B46" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>negara</t>
+          <t>menu</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47">
@@ -1175,15 +1175,15 @@
         <v>5</v>
       </c>
       <c r="B47" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>kocak</t>
+          <t>prabowo</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48">
@@ -1191,15 +1191,15 @@
         <v>6</v>
       </c>
       <c r="B48" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>jd</t>
+          <t>enak</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49">
@@ -1207,15 +1207,15 @@
         <v>7</v>
       </c>
       <c r="B49" t="n">
+        <v>2</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>corbuzier</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
         <v>7</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>racun</t>
-        </is>
-      </c>
-      <c r="D49" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="50">
@@ -1223,15 +1223,15 @@
         <v>8</v>
       </c>
       <c r="B50" t="n">
+        <v>2</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>banget</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
         <v>7</v>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>coba</t>
-        </is>
-      </c>
-      <c r="D50" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="51">
@@ -1239,15 +1239,15 @@
         <v>9</v>
       </c>
       <c r="B51" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>anakanak</t>
+          <t>gue</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52">
@@ -1255,15 +1255,15 @@
         <v>10</v>
       </c>
       <c r="B52" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>komen</t>
+          <t>video</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53">
@@ -1271,15 +1271,15 @@
         <v>11</v>
       </c>
       <c r="B53" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>enak</t>
+          <t>deddy</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54">
@@ -1287,15 +1287,15 @@
         <v>12</v>
       </c>
       <c r="B54" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>pas</t>
+          <t>suka</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55">
@@ -1303,15 +1303,15 @@
         <v>13</v>
       </c>
       <c r="B55" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>gmn</t>
+          <t>gua</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56">
@@ -1319,15 +1319,15 @@
         <v>14</v>
       </c>
       <c r="B56" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>jepang</t>
+          <t>azka</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57">
@@ -1335,15 +1335,15 @@
         <v>15</v>
       </c>
       <c r="B57" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>buka</t>
+          <t>nasi</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58">
@@ -1351,15 +1351,15 @@
         <v>16</v>
       </c>
       <c r="B58" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>mending</t>
+          <t>komentar</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59">
@@ -1367,15 +1367,15 @@
         <v>17</v>
       </c>
       <c r="B59" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>bilang</t>
+          <t>the</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60">
@@ -1383,15 +1383,15 @@
         <v>18</v>
       </c>
       <c r="B60" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>sakit</t>
+          <t>emang</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61">
@@ -1399,15 +1399,15 @@
         <v>19</v>
       </c>
       <c r="B61" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>biar</t>
+          <t>sekolah</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62">
@@ -1419,11 +1419,11 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>anak</t>
+          <t>anggar</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63">
@@ -1435,11 +1435,11 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>anggar</t>
+          <t>anak</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64">
@@ -1451,11 +1451,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>tuh</t>
+          <t>rakyat</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65">
@@ -1467,11 +1467,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>gizi</t>
+          <t>dana</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66">
@@ -1483,11 +1483,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>tuju</t>
+          <t>daerah</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67">
@@ -1499,11 +1499,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>miskin</t>
+          <t>orang</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68">
@@ -1515,11 +1515,11 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>daerah</t>
+          <t>sekolah</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69">
@@ -1531,11 +1531,11 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>lokal</t>
+          <t>gizi</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70">
@@ -1547,11 +1547,11 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>bagus</t>
+          <t>udah</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71">
@@ -1563,11 +1563,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>menu</t>
+          <t>bagus</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72">
@@ -1579,11 +1579,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>butuh</t>
+          <t>coba</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73">
@@ -1595,11 +1595,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>udah</t>
+          <t>duit</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74">
@@ -1611,11 +1611,11 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>coba</t>
+          <t>kantin</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75">
@@ -1627,11 +1627,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>masuk</t>
+          <t>tuju</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76">
@@ -1643,11 +1643,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>lihat</t>
+          <t>miskin</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77">
@@ -1659,11 +1659,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>utama</t>
+          <t>masuk</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78">
@@ -1675,11 +1675,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>orang</t>
+          <t>banget</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79">
@@ -1691,11 +1691,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>banget</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80">
@@ -1707,11 +1707,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>jd</t>
+          <t>mending</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81">
@@ -1723,11 +1723,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>beda</t>
+          <t>vendor</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82">
@@ -1735,15 +1735,15 @@
         <v>0</v>
       </c>
       <c r="B82" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>anak</t>
+          <t>prabowo</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83">
@@ -1751,15 +1751,15 @@
         <v>1</v>
       </c>
       <c r="B83" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>gizi</t>
+          <t>uang</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84">
@@ -1767,15 +1767,15 @@
         <v>2</v>
       </c>
       <c r="B84" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>prabowo</t>
+          <t>gizi</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85">
@@ -1783,11 +1783,11 @@
         <v>3</v>
       </c>
       <c r="B85" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>sekolah</t>
+          <t>bantu</t>
         </is>
       </c>
       <c r="D85" t="n">
@@ -1799,7 +1799,7 @@
         <v>4</v>
       </c>
       <c r="B86" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -1815,11 +1815,11 @@
         <v>5</v>
       </c>
       <c r="B87" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>indonesia</t>
+          <t>anak</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -1831,11 +1831,11 @@
         <v>6</v>
       </c>
       <c r="B88" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>gue</t>
+          <t>sekolah</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -1847,7 +1847,7 @@
         <v>7</v>
       </c>
       <c r="B89" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -1863,15 +1863,15 @@
         <v>8</v>
       </c>
       <c r="B90" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>nasi</t>
+          <t>indonesia</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91">
@@ -1879,11 +1879,11 @@
         <v>9</v>
       </c>
       <c r="B91" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>uang</t>
+          <t>perintah</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -1895,11 +1895,11 @@
         <v>10</v>
       </c>
       <c r="B92" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>potong</t>
+          <t>rakyat</t>
         </is>
       </c>
       <c r="D92" t="n">
@@ -1911,11 +1911,11 @@
         <v>11</v>
       </c>
       <c r="B93" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>anggar</t>
+          <t>negara</t>
         </is>
       </c>
       <c r="D93" t="n">
@@ -1927,11 +1927,11 @@
         <v>12</v>
       </c>
       <c r="B94" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>sehat</t>
+          <t>rp</t>
         </is>
       </c>
       <c r="D94" t="n">
@@ -1943,11 +1943,11 @@
         <v>13</v>
       </c>
       <c r="B95" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>menu</t>
+          <t>bayar</t>
         </is>
       </c>
       <c r="D95" t="n">
@@ -1959,11 +1959,11 @@
         <v>14</v>
       </c>
       <c r="B96" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>mas</t>
+          <t>dana</t>
         </is>
       </c>
       <c r="D96" t="n">
@@ -1975,15 +1975,15 @@
         <v>15</v>
       </c>
       <c r="B97" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>kaya</t>
+          <t>gas</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98">
@@ -1991,11 +1991,11 @@
         <v>16</v>
       </c>
       <c r="B98" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>dapet</t>
+          <t>kaya</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2007,11 +2007,11 @@
         <v>17</v>
       </c>
       <c r="B99" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>anakanak</t>
+          <t>dapet</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2023,11 +2023,11 @@
         <v>18</v>
       </c>
       <c r="B100" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>perintah</t>
+          <t>pajak</t>
         </is>
       </c>
       <c r="D100" t="n">
@@ -2039,975 +2039,15 @@
         <v>19</v>
       </c>
       <c r="B101" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>udah</t>
+          <t>potong</t>
         </is>
       </c>
       <c r="D101" t="n">
         <v>4</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B102" t="n">
-        <v>1</v>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>udah</t>
-        </is>
-      </c>
-      <c r="D102" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B103" t="n">
-        <v>1</v>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>butuh</t>
-        </is>
-      </c>
-      <c r="D103" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B104" t="n">
-        <v>1</v>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>anak</t>
-        </is>
-      </c>
-      <c r="D104" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B105" t="n">
-        <v>1</v>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>enak</t>
-        </is>
-      </c>
-      <c r="D105" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B106" t="n">
-        <v>1</v>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>anggar</t>
-        </is>
-      </c>
-      <c r="D106" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B107" t="n">
-        <v>1</v>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>gitu</t>
-        </is>
-      </c>
-      <c r="D107" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B108" t="n">
-        <v>1</v>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>dapet</t>
-        </is>
-      </c>
-      <c r="D108" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B109" t="n">
-        <v>1</v>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>orang</t>
-        </is>
-      </c>
-      <c r="D109" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B110" t="n">
-        <v>1</v>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>kuliah</t>
-        </is>
-      </c>
-      <c r="D110" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B111" t="n">
-        <v>1</v>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>nih</t>
-        </is>
-      </c>
-      <c r="D111" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B112" t="n">
-        <v>1</v>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>konsep</t>
-        </is>
-      </c>
-      <c r="D112" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B113" t="n">
-        <v>1</v>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>gizi</t>
-        </is>
-      </c>
-      <c r="D113" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B114" t="n">
-        <v>1</v>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>kenyang</t>
-        </is>
-      </c>
-      <c r="D114" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B115" t="n">
-        <v>1</v>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>nenek</t>
-        </is>
-      </c>
-      <c r="D115" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B116" t="n">
-        <v>1</v>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>moyang</t>
-        </is>
-      </c>
-      <c r="D116" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B117" t="n">
-        <v>1</v>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>eh</t>
-        </is>
-      </c>
-      <c r="D117" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B118" t="n">
-        <v>1</v>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>tu</t>
-        </is>
-      </c>
-      <c r="D118" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B119" t="n">
-        <v>1</v>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>uda</t>
-        </is>
-      </c>
-      <c r="D119" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B120" t="n">
-        <v>1</v>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>dibawain</t>
-        </is>
-      </c>
-      <c r="D120" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B121" t="n">
-        <v>1</v>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>bekal</t>
-        </is>
-      </c>
-      <c r="D121" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B122" t="n">
-        <v>3</v>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>perintah</t>
-        </is>
-      </c>
-      <c r="D122" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B123" t="n">
-        <v>3</v>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>gizi</t>
-        </is>
-      </c>
-      <c r="D123" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B124" t="n">
-        <v>3</v>
-      </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>indonesia</t>
-        </is>
-      </c>
-      <c r="D124" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B125" t="n">
-        <v>3</v>
-      </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>rumah</t>
-        </is>
-      </c>
-      <c r="D125" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B126" t="n">
-        <v>3</v>
-      </c>
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>anak</t>
-        </is>
-      </c>
-      <c r="D126" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B127" t="n">
-        <v>3</v>
-      </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>bikin</t>
-        </is>
-      </c>
-      <c r="D127" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B128" t="n">
-        <v>3</v>
-      </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>anakanak</t>
-        </is>
-      </c>
-      <c r="D128" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B129" t="n">
-        <v>3</v>
-      </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>banget</t>
-        </is>
-      </c>
-      <c r="D129" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B130" t="n">
-        <v>3</v>
-      </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>sekolah</t>
-        </is>
-      </c>
-      <c r="D130" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B131" t="n">
-        <v>3</v>
-      </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>sehat</t>
-        </is>
-      </c>
-      <c r="D131" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B132" t="n">
-        <v>3</v>
-      </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>menu</t>
-        </is>
-      </c>
-      <c r="D132" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B133" t="n">
-        <v>3</v>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>tuju</t>
-        </is>
-      </c>
-      <c r="D133" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B134" t="n">
-        <v>3</v>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>orang</t>
-        </is>
-      </c>
-      <c r="D134" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B135" t="n">
-        <v>3</v>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>keren</t>
-        </is>
-      </c>
-      <c r="D135" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B136" t="n">
-        <v>3</v>
-      </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>mantap</t>
-        </is>
-      </c>
-      <c r="D136" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B137" t="n">
-        <v>3</v>
-      </c>
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>miskin</t>
-        </is>
-      </c>
-      <c r="D137" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B138" t="n">
-        <v>3</v>
-      </c>
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>generasi</t>
-        </is>
-      </c>
-      <c r="D138" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B139" t="n">
-        <v>3</v>
-      </c>
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>anak2</t>
-        </is>
-      </c>
-      <c r="D139" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B140" t="n">
-        <v>3</v>
-      </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>sampe</t>
-        </is>
-      </c>
-      <c r="D140" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B141" t="n">
-        <v>3</v>
-      </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>nama</t>
-        </is>
-      </c>
-      <c r="D141" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B142" t="n">
-        <v>6</v>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>prabowo</t>
-        </is>
-      </c>
-      <c r="D142" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B143" t="n">
-        <v>6</v>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>anak</t>
-        </is>
-      </c>
-      <c r="D143" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B144" t="n">
-        <v>6</v>
-      </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>corbuzier</t>
-        </is>
-      </c>
-      <c r="D144" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B145" t="n">
-        <v>6</v>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>bicara</t>
-        </is>
-      </c>
-      <c r="D145" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B146" t="n">
-        <v>6</v>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>perintah</t>
-        </is>
-      </c>
-      <c r="D146" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B147" t="n">
-        <v>6</v>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>iya</t>
-        </is>
-      </c>
-      <c r="D147" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B148" t="n">
-        <v>6</v>
-      </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>deddy</t>
-        </is>
-      </c>
-      <c r="D148" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B149" t="n">
-        <v>6</v>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>psi</t>
-        </is>
-      </c>
-      <c r="D149" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B150" t="n">
-        <v>6</v>
-      </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>lihat</t>
-        </is>
-      </c>
-      <c r="D150" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B151" t="n">
-        <v>6</v>
-      </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D151" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B152" t="n">
-        <v>6</v>
-      </c>
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>indonesia</t>
-        </is>
-      </c>
-      <c r="D152" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B153" t="n">
-        <v>6</v>
-      </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>gw</t>
-        </is>
-      </c>
-      <c r="D153" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B154" t="n">
-        <v>6</v>
-      </c>
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>komenin</t>
-        </is>
-      </c>
-      <c r="D154" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B155" t="n">
-        <v>6</v>
-      </c>
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>banget</t>
-        </is>
-      </c>
-      <c r="D155" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B156" t="n">
-        <v>6</v>
-      </c>
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>ngeluh</t>
-        </is>
-      </c>
-      <c r="D156" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B157" t="n">
-        <v>6</v>
-      </c>
-      <c r="C157" t="inlineStr">
-        <is>
-          <t>enak</t>
-        </is>
-      </c>
-      <c r="D157" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B158" t="n">
-        <v>6</v>
-      </c>
-      <c r="C158" t="inlineStr">
-        <is>
-          <t>presiden</t>
-        </is>
-      </c>
-      <c r="D158" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B159" t="n">
-        <v>6</v>
-      </c>
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>bikin</t>
-        </is>
-      </c>
-      <c r="D159" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B160" t="n">
-        <v>6</v>
-      </c>
-      <c r="C160" t="inlineStr">
-        <is>
-          <t>mantan</t>
-        </is>
-      </c>
-      <c r="D160" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B161" t="n">
-        <v>6</v>
-      </c>
-      <c r="C161" t="inlineStr">
-        <is>
-          <t>dr</t>
-        </is>
-      </c>
-      <c r="D161" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>